<commit_message>
adds RVCAT to FN2 species code conversion
</commit_message>
<xml_diff>
--- a/data-raw/SPCShort2SPECIESRVCAT.xlsx
+++ b/data-raw/SPCShort2SPECIESRVCAT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/jeremy_holden_ontario_ca/Documents/Documents/R/lakeontario/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{5CAD2A63-89C1-4955-942B-DA4B0BE7884E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{17F1A04B-42D9-49AE-9844-21B490A0BBB9}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{5CAD2A63-89C1-4955-942B-DA4B0BE7884E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47997712-7099-4D91-865F-284809C215EE}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7BBD6B9C-923A-421F-9A55-29F38A987C72}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BBD6B9C-923A-421F-9A55-29F38A987C72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>SPC_SHORT</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>CoCar</t>
+  </si>
+  <si>
+    <t>Bloat</t>
+  </si>
+  <si>
+    <t>094</t>
   </si>
 </sst>
 </file>
@@ -529,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8D6633-9696-4983-AABC-5C9DF74C6035}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,8 +975,25 @@
         <v>186</v>
       </c>
     </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <v>204</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{034a106e-6316-442c-ad35-738afd673d2b}" enabled="1" method="Standard" siteId="{cddc1229-ac2a-4b97-b78a-0e5cacb5865c}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>